<commit_message>
Added time sheet for week 2015-11-16
</commit_message>
<xml_diff>
--- a/man/completed sheets/2015-11-16/Joshua Doyle.xlsx
+++ b/man/completed sheets/2015-11-16/Joshua Doyle.xlsx
@@ -49,21 +49,12 @@
     <t>Comments</t>
   </si>
   <si>
-    <t>Create an example task and populate fields</t>
-  </si>
-  <si>
-    <t>Design/Documentation/Code/Testing…etc</t>
-  </si>
-  <si>
     <t>abc123</t>
   </si>
   <si>
     <t>John Smith</t>
   </si>
   <si>
-    <t>I spend an extra 30 minutes trying to get a foo trying to communicate to a bar however I completed implementing foo within only 15 minutes. Text should autowrap on enter.</t>
-  </si>
-  <si>
     <t>Time Budgeted</t>
   </si>
   <si>
@@ -71,6 +62,15 @@
   </si>
   <si>
     <t>Design and Create Mock-up of User Interface</t>
+  </si>
+  <si>
+    <t>Created UI designs for all TaskerCLI windows</t>
+  </si>
+  <si>
+    <t>Design</t>
+  </si>
+  <si>
+    <t>This took longer than I expected it to due to doing this task using Micrsoft Office. This created difficulties in creating a representative design that took a long time to work around.</t>
   </si>
 </sst>
 </file>
@@ -471,7 +471,7 @@
       <pane xSplit="8" ySplit="2" topLeftCell="I3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomRight" activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -491,13 +491,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>2</v>
@@ -507,11 +507,11 @@
       </c>
       <c r="G1" s="4" t="str">
         <f>"Total hours accounted this week: " &amp;TEXT(I1, "hh:mm")</f>
-        <v>Total hours accounted this week: 01:30</v>
+        <v>Total hours accounted this week: 06:00</v>
       </c>
       <c r="I1" s="6">
         <f>SUM(F3:F100)</f>
-        <v>6.25E-2</v>
+        <v>0.25</v>
       </c>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
@@ -544,7 +544,7 @@
         <v>8</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>9</v>
@@ -552,28 +552,28 @@
     </row>
     <row r="3" spans="1:19" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="E3" s="10">
+        <v>42328</v>
+      </c>
+      <c r="F3" s="11">
+        <v>0.25</v>
+      </c>
+      <c r="G3" s="11">
+        <v>0.125</v>
+      </c>
+      <c r="H3" s="9" t="s">
         <v>17</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="10">
-        <v>42297</v>
-      </c>
-      <c r="F3" s="11">
-        <v>6.25E-2</v>
-      </c>
-      <c r="G3" s="11">
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="H3" s="9" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.35">

</xml_diff>